<commit_message>
Feat : Player 강화 구현
물리 공격력, 마법 공격력, 최대 체력, 시작 골드 강화 구현 및

던전 입장시 실행시켜서 스탯 적용시킬 함수 생성

Player -> SetUpgradeModifier
</commit_message>
<xml_diff>
--- a/Assets/Excel/Task/Upgrade/PlayerUpgradeDB_Sheet.xlsx
+++ b/Assets/Excel/Task/Upgrade/PlayerUpgradeDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\Task\Upgrade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D83192-737A-4541-AA48-0B3BDDC82888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2747CDEB-96D5-4980-BE30-18CE723D4411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{B7F7D38E-3A1A-46EA-8576-F6A7B1622EBD}"/>
+    <workbookView xWindow="-28680" yWindow="2235" windowWidth="25650" windowHeight="13155" xr2:uid="{B7F7D38E-3A1A-46EA-8576-F6A7B1622EBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>공격력 #N 증가</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -118,6 +118,30 @@
   </si>
   <si>
     <t>MagicAtk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력 #N 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시작 골드 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>골드 #N 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartGold</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxHP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최대 체력 증가</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -549,7 +573,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -745,6 +769,124 @@
         <v>25</v>
       </c>
     </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>50000002</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4">
+        <v>1234</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="J4" s="1">
+        <v>50</v>
+      </c>
+      <c r="K4">
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <v>150</v>
+      </c>
+      <c r="M4">
+        <v>200</v>
+      </c>
+      <c r="N4">
+        <v>250</v>
+      </c>
+      <c r="O4">
+        <v>10</v>
+      </c>
+      <c r="P4">
+        <v>20</v>
+      </c>
+      <c r="Q4">
+        <v>30</v>
+      </c>
+      <c r="R4">
+        <v>40</v>
+      </c>
+      <c r="S4">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>50000003</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5">
+        <v>1234</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1">
+        <v>50</v>
+      </c>
+      <c r="K5">
+        <v>100</v>
+      </c>
+      <c r="L5">
+        <v>150</v>
+      </c>
+      <c r="M5">
+        <v>200</v>
+      </c>
+      <c r="N5">
+        <v>250</v>
+      </c>
+      <c r="O5">
+        <v>30</v>
+      </c>
+      <c r="P5">
+        <v>60</v>
+      </c>
+      <c r="Q5">
+        <v>90</v>
+      </c>
+      <c r="R5">
+        <v>120</v>
+      </c>
+      <c r="S5">
+        <v>150</v>
+      </c>
+    </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
     </row>

</xml_diff>

<commit_message>
Refactor : 자잘한 수정
</commit_message>
<xml_diff>
--- a/Assets/Excel/Task/Upgrade/PlayerUpgradeDB_Sheet.xlsx
+++ b/Assets/Excel/Task/Upgrade/PlayerUpgradeDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\Task\Upgrade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121F6A22-B4EC-4323-8E7D-383CFB05B5A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA412900-D012-4897-B3CA-A5857FA1EA11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{B7F7D38E-3A1A-46EA-8576-F6A7B1622EBD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{B7F7D38E-3A1A-46EA-8576-F6A7B1622EBD}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -573,7 +573,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -668,7 +668,7 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <v>1234</v>
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -727,7 +727,7 @@
         <v>24</v>
       </c>
       <c r="F3">
-        <v>1234</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -786,7 +786,7 @@
         <v>29</v>
       </c>
       <c r="F4">
-        <v>1234</v>
+        <v>0</v>
       </c>
       <c r="G4">
         <v>0</v>
@@ -845,7 +845,7 @@
         <v>28</v>
       </c>
       <c r="F5">
-        <v>1234</v>
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>

</xml_diff>